<commit_message>
First MVC successful. Using form handling with @ModeAttribute annotation.
</commit_message>
<xml_diff>
--- a/Spring_interview_questions.xlsx
+++ b/Spring_interview_questions.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="904"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="904" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Configurations" sheetId="17" r:id="rId1"/>
@@ -7741,8 +7741,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8445,14 +8445,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8544,6 +8544,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -8578,6 +8579,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8753,23 +8755,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.140625" customWidth="1"/>
     <col min="4" max="4" width="52.42578125" customWidth="1"/>
     <col min="5" max="5" width="49.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
       <c r="D2" s="41" t="s">
@@ -8779,7 +8781,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="45">
+    <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="50" t="s">
         <v>139</v>
       </c>
@@ -8789,7 +8791,7 @@
       </c>
       <c r="E3" s="50"/>
     </row>
-    <row r="4" spans="2:5" ht="90">
+    <row r="4" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B4" s="52" t="s">
         <v>138</v>
       </c>
@@ -8801,7 +8803,7 @@
       </c>
       <c r="E4" s="50"/>
     </row>
-    <row r="5" spans="2:5" ht="165">
+    <row r="5" spans="2:5" ht="150" x14ac:dyDescent="0.25">
       <c r="B5" s="51" t="s">
         <v>146</v>
       </c>
@@ -8813,7 +8815,7 @@
       </c>
       <c r="E5" s="50"/>
     </row>
-    <row r="6" spans="2:5" ht="120">
+    <row r="6" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B6" s="50" t="s">
         <v>145</v>
       </c>
@@ -8823,7 +8825,7 @@
       <c r="D6" s="50"/>
       <c r="E6" s="50"/>
     </row>
-    <row r="7" spans="2:5" ht="105">
+    <row r="7" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B7" s="50" t="s">
         <v>148</v>
       </c>
@@ -8833,7 +8835,7 @@
       </c>
       <c r="E7" s="50"/>
     </row>
-    <row r="8" spans="2:5" ht="90">
+    <row r="8" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="51" t="s">
         <v>150</v>
       </c>
@@ -8845,7 +8847,7 @@
       </c>
       <c r="E8" s="50"/>
     </row>
-    <row r="9" spans="2:5" ht="150">
+    <row r="9" spans="2:5" ht="150" x14ac:dyDescent="0.25">
       <c r="B9" s="50" t="s">
         <v>153</v>
       </c>
@@ -8855,7 +8857,7 @@
       </c>
       <c r="E9" s="50"/>
     </row>
-    <row r="10" spans="2:5" ht="120">
+    <row r="10" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B10" s="51" t="s">
         <v>155</v>
       </c>
@@ -8865,7 +8867,7 @@
       </c>
       <c r="E10" s="50"/>
     </row>
-    <row r="11" spans="2:5" ht="150">
+    <row r="11" spans="2:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B11" s="50" t="s">
         <v>157</v>
       </c>
@@ -8877,7 +8879,7 @@
       </c>
       <c r="E11" s="50"/>
     </row>
-    <row r="12" spans="2:5" ht="120">
+    <row r="12" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B12" s="53" t="s">
         <v>160</v>
       </c>
@@ -8889,7 +8891,7 @@
       </c>
       <c r="E12" s="51"/>
     </row>
-    <row r="13" spans="2:5" ht="120">
+    <row r="13" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B13" s="51" t="s">
         <v>167</v>
       </c>
@@ -8901,7 +8903,7 @@
       </c>
       <c r="E13" s="51"/>
     </row>
-    <row r="14" spans="2:5" ht="270">
+    <row r="14" spans="2:5" ht="270" x14ac:dyDescent="0.25">
       <c r="B14" s="51" t="s">
         <v>173</v>
       </c>
@@ -8913,7 +8915,7 @@
       </c>
       <c r="E14" s="51"/>
     </row>
-    <row r="15" spans="2:5" ht="60">
+    <row r="15" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="51" t="s">
         <v>170</v>
       </c>
@@ -8925,7 +8927,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="240">
+    <row r="16" spans="2:5" ht="240" x14ac:dyDescent="0.25">
       <c r="B16" s="51" t="s">
         <v>176</v>
       </c>
@@ -8939,7 +8941,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="165">
+    <row r="17" spans="2:5" ht="165" x14ac:dyDescent="0.25">
       <c r="B17" s="51" t="s">
         <v>180</v>
       </c>
@@ -8953,7 +8955,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="210">
+    <row r="18" spans="2:5" ht="210" x14ac:dyDescent="0.25">
       <c r="B18" s="51" t="s">
         <v>187</v>
       </c>
@@ -8963,21 +8965,21 @@
       <c r="D18" s="51" t="s">
         <v>195</v>
       </c>
-      <c r="E18" s="65" t="s">
+      <c r="E18" s="64" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="30">
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="E19" s="64" t="s">
+      <c r="E19" s="63" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="30">
+    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="50"/>
       <c r="C20" s="50"/>
       <c r="D20" s="51" t="s">
@@ -8987,7 +8989,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="45">
+    <row r="21" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
       <c r="D21" s="51" t="s">
@@ -8997,55 +8999,55 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="50"/>
       <c r="C22" s="50"/>
       <c r="D22" s="50"/>
       <c r="E22" s="50"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
       <c r="E23" s="50"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="50"/>
       <c r="C24" s="50"/>
       <c r="D24" s="50"/>
       <c r="E24" s="50"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="50"/>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
       <c r="E25" s="50"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="50"/>
       <c r="C26" s="50"/>
       <c r="D26" s="50"/>
       <c r="E26" s="50"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
       <c r="E27" s="50"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="50"/>
       <c r="C28" s="50"/>
       <c r="D28" s="50"/>
       <c r="E28" s="50"/>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="50"/>
       <c r="C29" s="50"/>
       <c r="D29" s="50"/>
       <c r="E29" s="50"/>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="50"/>
       <c r="C30" s="50"/>
       <c r="D30" s="50"/>
@@ -9058,21 +9060,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.140625" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9083,7 +9085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="90">
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>67</v>
       </c>
@@ -9092,7 +9094,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="90">
+    <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>66</v>
       </c>
@@ -9101,7 +9103,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" ht="120">
+    <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>69</v>
       </c>
@@ -9110,7 +9112,7 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" ht="45">
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>71</v>
       </c>
@@ -9119,7 +9121,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="45">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>73</v>
       </c>
@@ -9128,7 +9130,7 @@
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" ht="180">
+    <row r="7" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>78</v>
       </c>
@@ -9137,7 +9139,7 @@
       </c>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>75</v>
       </c>
@@ -9146,44 +9148,44 @@
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="11"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="11"/>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9"/>
@@ -9194,14 +9196,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
@@ -9209,7 +9211,7 @@
     <col min="4" max="4" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9220,7 +9222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>80</v>
       </c>
@@ -9229,7 +9231,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="75">
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>109</v>
       </c>
@@ -9240,7 +9242,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="105">
+    <row r="4" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>82</v>
       </c>
@@ -9249,7 +9251,7 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" ht="90">
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>85</v>
       </c>
@@ -9258,7 +9260,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="45">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>91</v>
       </c>
@@ -9267,7 +9269,7 @@
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" ht="75">
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>93</v>
       </c>
@@ -9276,7 +9278,7 @@
       </c>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="105">
+    <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>119</v>
       </c>
@@ -9287,7 +9289,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="90">
+    <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>103</v>
       </c>
@@ -9298,7 +9300,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="195">
+    <row r="10" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>126</v>
       </c>
@@ -9309,72 +9311,72 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="11"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="11"/>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="11"/>
       <c r="C15" s="14"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="11"/>
       <c r="C16" s="14"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="11"/>
       <c r="C17" s="14"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="11"/>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="11"/>
       <c r="C19" s="14"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="11"/>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="11"/>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="11"/>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="11"/>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="11"/>
       <c r="C24" s="9"/>
@@ -9386,21 +9388,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9411,7 +9413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="135">
+    <row r="2" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>96</v>
       </c>
@@ -9420,7 +9422,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="120">
+    <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>95</v>
       </c>
@@ -9429,7 +9431,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" ht="45">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>98</v>
       </c>
@@ -9438,7 +9440,7 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" ht="75">
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>101</v>
       </c>
@@ -9447,7 +9449,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="270">
+    <row r="6" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>128</v>
       </c>
@@ -9456,7 +9458,7 @@
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" ht="195">
+    <row r="7" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>130</v>
       </c>
@@ -9465,12 +9467,12 @@
       </c>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9"/>
@@ -9481,21 +9483,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.140625" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9506,72 +9508,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="11"/>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="11"/>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="11"/>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="11"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="11"/>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="11"/>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="11"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="11"/>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
@@ -9582,21 +9584,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9607,7 +9609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="90">
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>106</v>
       </c>
@@ -9616,7 +9618,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="60">
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>107</v>
       </c>
@@ -9625,17 +9627,17 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="11"/>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="11"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="11"/>
       <c r="C6" s="9"/>
@@ -9646,26 +9648,26 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="47.5703125" customWidth="1"/>
@@ -9673,7 +9675,7 @@
     <col min="4" max="4" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickTop="1">
+    <row r="1" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
@@ -9684,7 +9686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="75">
+    <row r="2" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
@@ -9693,7 +9695,7 @@
       </c>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="2:4" ht="300">
+    <row r="3" spans="2:4" ht="330" x14ac:dyDescent="0.25">
       <c r="B3" s="44" t="s">
         <v>5</v>
       </c>
@@ -9702,7 +9704,7 @@
       </c>
       <c r="D3" s="40"/>
     </row>
-    <row r="4" spans="2:4" ht="255">
+    <row r="4" spans="2:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B4" s="42" t="s">
         <v>4</v>
       </c>
@@ -9711,7 +9713,7 @@
       </c>
       <c r="D4" s="40"/>
     </row>
-    <row r="5" spans="2:4" ht="105">
+    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
         <v>112</v>
       </c>
@@ -9720,7 +9722,7 @@
       </c>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="2:4" ht="30">
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="49" t="s">
         <v>59</v>
       </c>
@@ -9729,7 +9731,7 @@
       </c>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="2:4" ht="90">
+    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="48" t="s">
         <v>60</v>
       </c>
@@ -9738,7 +9740,7 @@
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="2:4" ht="60">
+    <row r="8" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="28" t="s">
         <v>49</v>
       </c>
@@ -9747,7 +9749,7 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="2:4" ht="225">
+    <row r="9" spans="2:4" ht="225" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>122</v>
       </c>
@@ -9758,7 +9760,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="255">
+    <row r="10" spans="2:4" ht="285" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
         <v>124</v>
       </c>
@@ -9767,7 +9769,7 @@
       </c>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>132</v>
       </c>
@@ -9787,21 +9789,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="57.42578125" customWidth="1"/>
     <col min="3" max="3" width="63.140625" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickTop="1">
+    <row r="1" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B1" s="57" t="s">
         <v>0</v>
       </c>
@@ -9812,7 +9814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="165">
+    <row r="2" spans="2:4" ht="165" x14ac:dyDescent="0.25">
       <c r="B2" s="49" t="s">
         <v>7</v>
       </c>
@@ -9821,7 +9823,7 @@
       </c>
       <c r="D2" s="56"/>
     </row>
-    <row r="3" spans="2:4" ht="135">
+    <row r="3" spans="2:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B3" s="44" t="s">
         <v>8</v>
       </c>
@@ -9830,35 +9832,35 @@
       </c>
       <c r="D3" s="56"/>
     </row>
-    <row r="4" spans="2:4" ht="31.5">
+    <row r="4" spans="2:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B4" s="54" t="s">
         <v>163</v>
       </c>
       <c r="C4" s="51"/>
       <c r="D4" s="55"/>
     </row>
-    <row r="5" spans="2:4" ht="47.25" customHeight="1">
-      <c r="B5" s="63" t="s">
+    <row r="5" spans="2:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="63"/>
+      <c r="C5" s="65"/>
       <c r="D5" s="55"/>
     </row>
-    <row r="6" spans="2:4" ht="30.75" customHeight="1">
-      <c r="B6" s="63" t="s">
+    <row r="6" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="65" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="63"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="55"/>
     </row>
-    <row r="7" spans="2:4" ht="33.75" customHeight="1">
-      <c r="B7" s="63" t="s">
+    <row r="7" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="65" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="63"/>
+      <c r="C7" s="65"/>
       <c r="D7" s="55"/>
     </row>
-    <row r="8" spans="2:4" ht="150">
+    <row r="8" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B8" s="44" t="s">
         <v>11</v>
       </c>
@@ -9867,7 +9869,7 @@
       </c>
       <c r="D8" s="40"/>
     </row>
-    <row r="9" spans="2:4" ht="60">
+    <row r="9" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="44" t="s">
         <v>13</v>
       </c>
@@ -9876,7 +9878,7 @@
       </c>
       <c r="D9" s="56"/>
     </row>
-    <row r="10" spans="2:4" ht="135">
+    <row r="10" spans="2:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B10" s="62" t="s">
         <v>15</v>
       </c>
@@ -9885,18 +9887,18 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="48"/>
       <c r="C11" s="11"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="2:4" ht="15.75" thickBot="1">
+    <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="2:4" ht="15.75" thickTop="1"/>
-    <row r="14" spans="2:4">
+    <row r="13" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
         <v>10</v>
       </c>
@@ -9912,21 +9914,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.42578125" style="26" customWidth="1"/>
     <col min="2" max="2" width="71" customWidth="1"/>
     <col min="3" max="3" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9937,7 +9939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>17</v>
       </c>
@@ -9948,7 +9950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>20</v>
       </c>
@@ -9957,126 +9959,126 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="11"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="11"/>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="11"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="11"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="11"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="11"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="11"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="11"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="11"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="11"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="11"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="11"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="11"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="11"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="11"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="11"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="11"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="11"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="11"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1">
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="12"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickTop="1"/>
+    <row r="25" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.140625" customWidth="1"/>
@@ -10085,7 +10087,7 @@
     <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10096,7 +10098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>22</v>
       </c>
@@ -10105,7 +10107,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="165">
+    <row r="3" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>116</v>
       </c>
@@ -10114,7 +10116,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" ht="240">
+    <row r="4" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>88</v>
       </c>
@@ -10123,168 +10125,168 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="11"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="11"/>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="11"/>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="11"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="11"/>
       <c r="C13" s="14"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="11"/>
       <c r="C14" s="14"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="11"/>
       <c r="C15" s="14"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="11"/>
       <c r="C17" s="14"/>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="11"/>
       <c r="C18" s="14"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="11"/>
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="11"/>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="11"/>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="11"/>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="11"/>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="11"/>
       <c r="C24" s="9"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="11"/>
       <c r="C25" s="9"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="11"/>
       <c r="C26" s="9"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="11"/>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="11"/>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="11"/>
       <c r="C29" s="9"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="11"/>
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
       <c r="B31" s="17"/>
       <c r="C31" s="18"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="17"/>
       <c r="C32" s="18"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="B33" s="17"/>
       <c r="C33" s="18"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="27"/>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="27"/>
       <c r="B35" s="17"/>
       <c r="C35" s="18"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1">
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="12"/>
       <c r="C36" s="10"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickTop="1"/>
+    <row r="37" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10292,21 +10294,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10317,7 +10319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>27</v>
       </c>
@@ -10326,7 +10328,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="120">
+    <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
@@ -10335,7 +10337,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" ht="75">
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>29</v>
       </c>
@@ -10344,14 +10346,14 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="270">
+    <row r="6" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>32</v>
       </c>
@@ -10362,7 +10364,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="195">
+    <row r="7" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>34</v>
       </c>
@@ -10373,7 +10375,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="132" customHeight="1">
+    <row r="8" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>114</v>
       </c>
@@ -10382,7 +10384,7 @@
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3" ht="405">
+    <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>37</v>
       </c>
@@ -10391,7 +10393,7 @@
       </c>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="75">
+    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>39</v>
       </c>
@@ -10400,7 +10402,7 @@
       </c>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:3" ht="195">
+    <row r="11" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>41</v>
       </c>
@@ -10409,17 +10411,17 @@
       </c>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="11"/>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="19"/>
@@ -10430,21 +10432,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.140625" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -10455,7 +10457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="75">
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>90</v>
       </c>
@@ -10464,7 +10466,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="345">
+    <row r="3" spans="1:3" ht="375" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>43</v>
       </c>
@@ -10473,7 +10475,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" ht="135">
+    <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>45</v>
       </c>
@@ -10482,7 +10484,7 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" ht="45">
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>52</v>
       </c>
@@ -10491,38 +10493,38 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="11"/>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32"/>
       <c r="B7" s="33"/>
       <c r="C7" s="34"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickTop="1"/>
+    <row r="8" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10533,7 +10535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="75">
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>53</v>
       </c>
@@ -10542,7 +10544,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="60">
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>55</v>
       </c>
@@ -10551,7 +10553,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" ht="75">
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>57</v>
       </c>
@@ -10560,7 +10562,7 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:3" ht="270">
+    <row r="5" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>117</v>
       </c>
@@ -10569,12 +10571,12 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
       <c r="B6" s="11"/>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
       <c r="B7" s="11"/>
       <c r="C7" s="9"/>
@@ -10585,21 +10587,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="71.42578125" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10610,7 +10612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>62</v>
       </c>
@@ -10619,7 +10621,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="300">
+    <row r="3" spans="1:3" ht="300" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>64</v>
       </c>
@@ -10628,62 +10630,62 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="11"/>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="11"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="11"/>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="11"/>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="11"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="11"/>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>

</xml_diff>